<commit_message>
nova analise dos normais
</commit_message>
<xml_diff>
--- a/Projeto/Geração das Amostras/excel/planilha_1.xlsx
+++ b/Projeto/Geração das Amostras/excel/planilha_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="54">
   <si>
     <t>exam_id</t>
   </si>
@@ -33,28 +33,151 @@
     <t>Nenhuma</t>
   </si>
   <si>
+    <t>Não</t>
+  </si>
+  <si>
     <t>Possível interferência em aVF e V5</t>
   </si>
   <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Possível interferência em D3. Boderline para bradicardia sinusal.</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>Sobrecarga ventricular esquerda, associada a bradicardia sinusal</t>
+  </si>
+  <si>
+    <t>RBBB</t>
+  </si>
+  <si>
+    <t>BRD com alteração secundária da repolarização. Preenche critérios para sobrecarga ventricular esquerda.</t>
+  </si>
+  <si>
     <t>Outra</t>
   </si>
   <si>
-    <t>Não</t>
-  </si>
-  <si>
-    <t>Taqj</t>
+    <t>Sobrecarga ventricular esquerda.</t>
   </si>
   <si>
     <t>AF</t>
   </si>
   <si>
+    <t>Possível extrassístole ou interferência, visualizada no início das derivações.</t>
+  </si>
+  <si>
+    <t>Extrassístole ventricular</t>
+  </si>
+  <si>
+    <t>Morfologia de BRD em precordias.</t>
+  </si>
+  <si>
+    <t>arritmia sinusal</t>
+  </si>
+  <si>
+    <t>Presença de extrassístole ventricular</t>
+  </si>
+  <si>
+    <t>Boderline para taquicardia sinsusal</t>
+  </si>
+  <si>
+    <t>LBBB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interferência </t>
+  </si>
+  <si>
+    <t>Boderline para BRD, QRS próximo de 120 ms</t>
+  </si>
+  <si>
+    <t>Sobrecarga atrial direita</t>
+  </si>
+  <si>
+    <t>Lesão com supradesnivelamento de ST em parede septal.</t>
+  </si>
+  <si>
+    <t>IAM antigo em parede septal. Lesão em atividade em parede antero-septal.</t>
+  </si>
+  <si>
+    <t>Interferência</t>
+  </si>
+  <si>
+    <t>Possível IAM antigo.</t>
+  </si>
+  <si>
+    <t>Extrassistole ventricular trigeminada</t>
+  </si>
+  <si>
+    <t>Isquemia miocárdica em paredes inferior e lateral. Presença de duas extrassístole supraventriculares.</t>
+  </si>
+  <si>
+    <t>Flutter atrial</t>
+  </si>
+  <si>
+    <t>Taquicardia atrial multifocal</t>
+  </si>
+  <si>
+    <t>Lesão com supradesnivelamento de ST em parede septal. Necrose em parede antero-septal.</t>
+  </si>
+  <si>
     <t>Arritmia sinusal</t>
   </si>
   <si>
-    <t>LBBB</t>
-  </si>
-  <si>
-    <t>Interferência</t>
+    <t>Lesão com supra de ST em parede antero-septal</t>
+  </si>
+  <si>
+    <t>Lesão com supra de ST em parede antero-septal e presença de extrassístole ventricular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Não </t>
+  </si>
+  <si>
+    <t>Não possível ver P em D2</t>
+  </si>
+  <si>
+    <t>Possível alteração de repolarização ou interferência</t>
+  </si>
+  <si>
+    <t>Possível interferência</t>
+  </si>
+  <si>
+    <t>Arritmia sinusal, limítrofe com bradicardia sinusal e normalidade</t>
+  </si>
+  <si>
+    <t>1dAVB</t>
+  </si>
+  <si>
+    <t>BAV de 1° grau, limítrofe com interferência</t>
+  </si>
+  <si>
+    <t>Isquemia de parede antero-septal</t>
+  </si>
+  <si>
+    <t>Necrose de parede septal, com lesão em atividade em parede antero-septal</t>
+  </si>
+  <si>
+    <t>Possivel isquemia em parede lateral</t>
+  </si>
+  <si>
+    <t>Possível arritmia sinusal ou normalidade</t>
+  </si>
+  <si>
+    <t>Lesão em parede antero-septal. Presença de sobrecarga atrial direita</t>
+  </si>
+  <si>
+    <t>Lesão em parede septal. Limítrofe para BRD</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Possível BRD. Sem visualização de V1</t>
+  </si>
+  <si>
+    <t>Limitrofe para BAV 1°</t>
   </si>
 </sst>
 </file>
@@ -80,12 +203,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -108,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -119,6 +248,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -363,108 +493,205 @@
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
         <v>2303.0</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
         <v>15542.0</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
         <v>18560.0</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
         <v>33661.0</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
         <v>41605.0</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
         <v>42054.0</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
         <v>52425.0</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
         <v>54398.0</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
         <v>56897.0</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
         <v>59396.0</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
         <v>60084.0</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
         <v>61018.0</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
         <v>62906.0</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
         <v>66896.0</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
@@ -484,15 +711,26 @@
       <c r="A19" s="2">
         <v>69378.0</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
         <v>84237.0</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2">
@@ -519,8 +757,12 @@
       <c r="A24" s="2">
         <v>103188.0</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2">
@@ -533,419 +775,735 @@
       <c r="A26" s="2">
         <v>104785.0</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2">
         <v>117460.0</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="B27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2">
         <v>117476.0</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="B28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2">
         <v>130282.0</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="B29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2">
         <v>134860.0</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="B30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2">
         <v>136677.0</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="2">
         <v>139887.0</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="2">
         <v>144629.0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="2">
         <v>150032.0</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="B34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="2">
         <v>161345.0</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="B35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="2">
         <v>177690.0</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="B36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="2">
         <v>183999.0</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="B37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="2">
         <v>185119.0</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="B38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="2">
         <v>204565.0</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="2">
         <v>205491.0</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2">
         <v>209602.0</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="B41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="2">
         <v>212673.0</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="B42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="2">
         <v>213924.0</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="B43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="2">
         <v>215469.0</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="B44" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="2">
         <v>219348.0</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="B45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="2">
         <v>229965.0</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="B46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="2">
         <v>231711.0</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="2">
         <v>233324.0</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="B48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="2">
         <v>236637.0</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="B49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="2">
         <v>238471.0</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="B50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="2">
         <v>250367.0</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="B51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="2">
         <v>255536.0</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="2">
         <v>257722.0</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="B53" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="2">
         <v>269344.0</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="B54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="2">
         <v>270359.0</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="B55" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="2">
         <v>270378.0</v>
       </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="B56" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="2">
         <v>276380.0</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="B57" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="2">
         <v>276901.0</v>
       </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="B58" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="2">
         <v>277965.0</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="B59" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="2">
         <v>279614.0</v>
       </c>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="B60" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="2">
         <v>298791.0</v>
       </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="B61" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="2">
         <v>315213.0</v>
       </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="B62" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="2">
         <v>317271.0</v>
       </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="B63" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="2">
         <v>321228.0</v>
       </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="B64" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="2">
         <v>336003.0</v>
       </c>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+      <c r="B65" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="2">
         <v>338057.0</v>
       </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+      <c r="B66" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="2">
         <v>340180.0</v>
       </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
+      <c r="B67" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="2">
         <v>346776.0</v>
       </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="B68" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="2">
         <v>350152.0</v>
       </c>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="B69" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="2">
+      <c r="A70" s="4">
         <v>354285.0</v>
       </c>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="4"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="4"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="4"/>
+      <c r="U70" s="4"/>
+      <c r="V70" s="4"/>
+      <c r="W70" s="4"/>
+      <c r="X70" s="4"/>
+      <c r="Y70" s="4"/>
+      <c r="Z70" s="4"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="2">
         <v>367932.0</v>
       </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
+      <c r="B71" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="2">
         <v>368755.0</v>
       </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
+      <c r="B72" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="2">
         <v>385667.0</v>
       </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
+      <c r="B73" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="2">
         <v>385870.0</v>
       </c>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
+      <c r="B74" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="2">
         <v>421486.0</v>
       </c>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
+      <c r="B75" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="2">
         <v>439867.0</v>
       </c>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
+      <c r="B76" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="2">
         <v>476595.0</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="2">
         <v>483034.0</v>
       </c>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
+      <c r="B78" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="2">
         <v>484984.0</v>
       </c>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
+      <c r="B79" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="2">
         <v>485287.0</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="2">
         <v>489846.0</v>
       </c>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
+      <c r="B81" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="B82" s="2"/>

</xml_diff>